<commit_message>
formatted ambiguity excel file
</commit_message>
<xml_diff>
--- a/Postprocessing_Ambiguity/Ambiguity.xlsx
+++ b/Postprocessing_Ambiguity/Ambiguity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dario\Documents\SemThes\Postprocessing_Ambiguity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dario\Documents\0_Github_Projects\SemThes\Postprocessing_Ambiguity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D74503-AA5C-44F0-A4D2-E7F05B4672D7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE3224D-A076-4835-A206-E0E9BDDC033B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17025" activeTab="3" xr2:uid="{91B92DB0-04EC-4F95-AF3A-3AC6549801F8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17025" activeTab="2" xr2:uid="{91B92DB0-04EC-4F95-AF3A-3AC6549801F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Blue channel" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -87,12 +94,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2478,1014 +2494,1028 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209472AB-72EB-4765-A096-A1DF736EDF13}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.85546875" defaultRowHeight="42.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.85546875" style="5"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="5">
         <v>0.5</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="5">
         <v>0.5</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="5">
         <v>0.5</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="5">
         <v>0.5</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="5">
         <v>0.53300000000000003</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="5">
         <v>0.53300000000000003</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="5">
         <v>0.53300000000000003</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="5">
         <v>0.53300000000000003</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="5">
         <v>0.56599999999999995</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="5">
         <v>0.56599999999999995</v>
       </c>
-      <c r="M1">
+      <c r="M1" s="5">
         <v>0.56599999999999995</v>
       </c>
-      <c r="N1">
+      <c r="N1" s="5">
         <v>0.56599999999999995</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="5">
         <v>0.6</v>
       </c>
-      <c r="P1">
+      <c r="P1" s="5">
         <v>0.6</v>
       </c>
-      <c r="Q1">
+      <c r="Q1" s="5">
         <v>0.6</v>
       </c>
-      <c r="R1">
+      <c r="R1" s="5">
         <v>0.6</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>28</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>30</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="5">
         <v>32</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="5">
         <v>34</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="5">
         <v>28</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="5">
         <v>30</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="5">
         <v>32</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="5">
         <v>34</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="5">
         <v>28</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="5">
         <v>30</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="5">
         <v>32</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="5">
         <v>34</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="5">
         <v>28</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="5">
         <v>30</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="5">
         <v>32</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="5">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
         <v>0.5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>28</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
         <v>662.83</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="7">
         <v>2542.27</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="7">
         <v>5652.02</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="6">
         <v>605.44000000000005</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="7">
         <v>2579.4699999999998</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="7">
         <v>5927.63</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="7">
         <v>10611.45</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="7">
         <v>2315.6799999999998</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="7">
         <v>5766.81</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="7">
         <v>10697.4</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="7">
         <v>17035.84</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="7">
         <v>5207.45</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="7">
         <v>10341.9</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="7">
         <v>17013.64</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="7">
         <v>25184.45</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>0.5</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>30</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="6">
         <v>662.83</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="D4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
         <v>651.69000000000005</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="7">
         <v>2519.58</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="6">
         <v>16.32</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="6">
         <v>670.27</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="7">
         <v>2705.8</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="7">
         <v>6094.17</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="6">
         <v>540.41</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="7">
         <v>2600</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="7">
         <v>6159.05</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="7">
         <v>11156.71</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="7">
         <v>2226.5300000000002</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="7">
         <v>5889.85</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="7">
         <v>11138.29</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="7">
         <v>17915.490000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>0.5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>32</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="7">
         <v>2542.27</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="6">
         <v>651.69000000000005</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="E5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
         <v>651.80999999999995</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="6">
         <v>710.09</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="6">
         <v>13.7</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="6">
         <v>747.66</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="7">
         <v>2842.69</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="6">
         <v>24.29</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="6">
         <v>692.36</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="7">
         <v>2887.34</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="7">
         <v>6543.03</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O5" s="6">
         <v>510.41</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="7">
         <v>2705.68</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="7">
         <v>6531.66</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="7">
         <v>11917.97</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>0.5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>34</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="7">
         <v>5652.02</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="7">
         <v>2519.58</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="6">
         <v>651.80999999999995</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="F6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
         <v>2634.8</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="6">
         <v>633.17999999999995</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="6">
         <v>21.59</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="6">
         <v>818.09</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="6">
         <v>773.82</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="6">
         <v>21.24</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="6">
         <v>844.75</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="7">
         <v>3150.54</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="6">
         <v>26.82</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="6">
         <v>747.51</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="7">
         <v>3141.09</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6" s="7">
         <v>7123.87</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>0.53300000000000003</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="5">
         <v>28</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="6">
         <v>605.44000000000005</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="6">
         <v>16.32</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="6">
         <v>710.09</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="7">
         <v>2634.8</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
+      <c r="G7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
         <v>729.41</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="7">
         <v>2825.43</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="7">
         <v>6272.75</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="6">
         <v>593.22</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="7">
         <v>2716.55</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="7">
         <v>6336.8</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="7">
         <v>11396.57</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="7">
         <v>2334.4299999999998</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="7">
         <v>6063.67</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="Q7" s="7">
         <v>11378.49</v>
       </c>
-      <c r="R7" s="2">
+      <c r="R7" s="7">
         <v>18218.990000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
         <v>0.53300000000000003</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>30</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="7">
         <v>2579.4699999999998</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="6">
         <v>670.27</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="6">
         <v>13.7</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="6">
         <v>633.17999999999995</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="6">
         <v>729.41</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
+      <c r="H8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="6">
         <v>727.25</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="7">
         <v>2803.51</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="6">
         <v>23.06</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="6">
         <v>673.13</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="7">
         <v>2848.48</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="7">
         <v>6486.65</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="6">
         <v>492.31</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="7">
         <v>2666.66</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="Q8" s="7">
         <v>6472.22</v>
       </c>
-      <c r="R8" s="2">
+      <c r="R8" s="7">
         <v>11840.16</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
         <v>0.53300000000000003</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <v>32</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="7">
         <v>5927.63</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="7">
         <v>2705.8</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="6">
         <v>747.66</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="6">
         <v>21.59</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="7">
         <v>2825.43</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="6">
         <v>727.25</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1">
+      <c r="I9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="6">
         <v>718.57</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="6">
         <v>878.26</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="6">
         <v>17.170000000000002</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="6">
         <v>741.12</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="7">
         <v>2950.64</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9" s="6">
         <v>42.53</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P9" s="6">
         <v>650.79999999999995</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="Q9" s="7">
         <v>2942.08</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R9" s="7">
         <v>6822.53</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
         <v>0.53300000000000003</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>34</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="7">
         <v>10611.45</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="7">
         <v>6094.17</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="7">
         <v>2842.69</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="6">
         <v>818.09</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="7">
         <v>6272.75</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="7">
         <v>2803.51</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="6">
         <v>718.57</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2">
+      <c r="J10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
         <v>3094.88</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="6">
         <v>774.97</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="6">
         <v>16.39</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="6">
         <v>803.3</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O10" s="6">
         <v>999.59</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P10" s="6">
         <v>20.12</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="Q10" s="6">
         <v>798.94</v>
       </c>
-      <c r="R10" s="2">
+      <c r="R10" s="7">
         <v>3197.51</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
         <v>0.56599999999999995</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="5">
         <v>28</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="7">
         <v>2315.6799999999998</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="6">
         <v>540.41</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="6">
         <v>24.29</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="6">
         <v>773.82</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="6">
         <v>593.22</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="6">
         <v>23.06</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="6">
         <v>878.26</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="7">
         <v>3094.88</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L11" s="1">
+      <c r="K11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="6">
         <v>817.86</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="7">
         <v>3141.8</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="7">
         <v>6924.49</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="6">
         <v>616.22</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11" s="7">
         <v>2950.23</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="Q11" s="7">
         <v>6908.86</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R11" s="7">
         <v>12428.62</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
         <v>0.56599999999999995</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <v>30</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="7">
         <v>5766.81</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="7">
         <v>2600</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="6">
         <v>692.36</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="6">
         <v>21.24</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="7">
         <v>2716.55</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="6">
         <v>673.13</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="6">
         <v>17.170000000000002</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="6">
         <v>774.97</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="6">
         <v>817.86</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M12" s="1">
+      <c r="L12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="6">
         <v>798.35</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="7">
         <v>3065.95</v>
       </c>
-      <c r="O12" s="1">
+      <c r="O12" s="6">
         <v>29.64</v>
       </c>
-      <c r="P12" s="1">
+      <c r="P12" s="6">
         <v>704.43</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="Q12" s="7">
         <v>3056.16</v>
       </c>
-      <c r="R12" s="2">
+      <c r="R12" s="7">
         <v>6999.33</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
         <v>0.56599999999999995</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="5">
         <v>32</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="7">
         <v>10697.4</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="7">
         <v>6159.05</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="7">
         <v>2887.34</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="6">
         <v>844.75</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="7">
         <v>6336.8</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="7">
         <v>2848.48</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="6">
         <v>741.12</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="6">
         <v>16.39</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="7">
         <v>3141.8</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="6">
         <v>798.35</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N13" s="1">
+      <c r="M13" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="6">
         <v>779.03</v>
       </c>
-      <c r="O13" s="2">
+      <c r="O13" s="7">
         <v>1027.22</v>
       </c>
-      <c r="P13" s="1">
+      <c r="P13" s="6">
         <v>19.72</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="Q13" s="6">
         <v>774.4</v>
       </c>
-      <c r="R13" s="2">
+      <c r="R13" s="7">
         <v>3151.18</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
         <v>0.56599999999999995</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="5">
         <v>34</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="7">
         <v>17035.84</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="7">
         <v>11156.71</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="7">
         <v>6543.03</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="7">
         <v>3150.54</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="7">
         <v>11396.57</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="7">
         <v>6486.65</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="7">
         <v>2950.64</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="6">
         <v>803.3</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="7">
         <v>6924.49</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="7">
         <v>3065.95</v>
       </c>
-      <c r="M14" s="1">
+      <c r="M14" s="6">
         <v>779.03</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O14" s="2">
+      <c r="N14" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" s="7">
         <v>3502.18</v>
       </c>
-      <c r="P14" s="1">
+      <c r="P14" s="6">
         <v>879.1</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="Q14" s="6">
         <v>14.16</v>
       </c>
-      <c r="R14" s="1">
+      <c r="R14" s="6">
         <v>845.04</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
         <v>0.6</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="5">
         <v>28</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="7">
         <v>5207.45</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="7">
         <v>2226.5300000000002</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="6">
         <v>510.41</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="6">
         <v>26.82</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="7">
         <v>2334.4299999999998</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="6">
         <v>492.31</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="6">
         <v>42.53</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="6">
         <v>999.59</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="6">
         <v>616.22</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15" s="6">
         <v>29.64</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="7">
         <v>1027.22</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="7">
         <v>3502.18</v>
       </c>
-      <c r="O15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P15" s="1">
+      <c r="O15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P15" s="6">
         <v>918.66</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="Q15" s="7">
         <v>3490.97</v>
       </c>
-      <c r="R15" s="2">
+      <c r="R15" s="7">
         <v>7650.08</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
         <v>0.6</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="5">
         <v>30</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="7">
         <v>10341.9</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="7">
         <v>5889.85</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="7">
         <v>2705.68</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="6">
         <v>747.51</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="7">
         <v>6063.67</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="7">
         <v>2666.66</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="6">
         <v>650.79999999999995</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="6">
         <v>20.12</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="7">
         <v>2950.23</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="6">
         <v>704.43</v>
       </c>
-      <c r="M16" s="1">
+      <c r="M16" s="6">
         <v>19.72</v>
       </c>
-      <c r="N16" s="1">
+      <c r="N16" s="6">
         <v>879.1</v>
       </c>
-      <c r="O16" s="1">
+      <c r="O16" s="6">
         <v>918.66</v>
       </c>
-      <c r="P16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="1">
+      <c r="P16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="6">
         <v>873.24</v>
       </c>
-      <c r="R16" s="2">
+      <c r="R16" s="7">
         <v>3351.37</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
         <v>0.6</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="5">
         <v>32</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="7">
         <v>17013.64</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="7">
         <v>11138.29</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="7">
         <v>6531.66</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="7">
         <v>3141.09</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="7">
         <v>11378.49</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="7">
         <v>6472.22</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="7">
         <v>2942.08</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="6">
         <v>798.94</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="7">
         <v>6908.86</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="7">
         <v>3056.16</v>
       </c>
-      <c r="M17" s="1">
+      <c r="M17" s="6">
         <v>774.4</v>
       </c>
-      <c r="N17" s="1">
+      <c r="N17" s="6">
         <v>14.16</v>
       </c>
-      <c r="O17" s="2">
+      <c r="O17" s="7">
         <v>3490.97</v>
       </c>
-      <c r="P17" s="1">
+      <c r="P17" s="6">
         <v>873.24</v>
       </c>
-      <c r="Q17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R17" s="1">
+      <c r="Q17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" s="6">
         <v>849.07</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
         <v>0.6</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="5">
         <v>34</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="7">
         <v>25184.45</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="7">
         <v>17915.490000000002</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="7">
         <v>11917.97</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="7">
         <v>7123.87</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="7">
         <v>18218.990000000002</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="7">
         <v>11840.16</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="7">
         <v>6822.53</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="7">
         <v>3197.51</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="7">
         <v>12428.62</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="7">
         <v>6999.33</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M18" s="7">
         <v>3151.18</v>
       </c>
-      <c r="N18" s="1">
+      <c r="N18" s="6">
         <v>845.04</v>
       </c>
-      <c r="O18" s="2">
+      <c r="O18" s="7">
         <v>7650.08</v>
       </c>
-      <c r="P18" s="2">
+      <c r="P18" s="7">
         <v>3351.37</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="Q18" s="6">
         <v>849.07</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="R18" s="6" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3503,6 +3533,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="60" orientation="landscape" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3510,7 +3541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B41B264-21C3-4259-AC5E-A19DF24612E5}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>